<commit_message>
Corrige acentuacao na Area de Experimentacao (Sprint 1, 2 e 3)
</commit_message>
<xml_diff>
--- a/Sprint3/Area_de_Experimentacao.xlsx
+++ b/Sprint3/Area_de_Experimentacao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sprint 1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -54,31 +54,31 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <sz val="16"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <sz val="12"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <sz val="14"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <name val="Calibri"/>
       <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-    </font>
-    <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -113,24 +113,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBDD7EE"/>
         <bgColor rgb="FFBDD7EE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFEB9C"/>
-        <bgColor rgb="00FFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -177,7 +159,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -188,27 +169,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,28 +562,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" style="13" min="1" max="1"/>
-    <col width="96.28515625" bestFit="1" customWidth="1" style="13" min="2" max="2"/>
-    <col width="55" customWidth="1" style="13" min="3" max="3"/>
-    <col width="25" customWidth="1" style="13" min="4" max="5"/>
-    <col width="15" customWidth="1" style="13" min="6" max="7"/>
+    <col width="22" customWidth="1" style="12" min="1" max="1"/>
+    <col width="96.28515625" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="55" customWidth="1" style="12" min="3" max="3"/>
+    <col width="25" customWidth="1" style="12" min="4" max="5"/>
+    <col width="15" customWidth="1" style="12" min="6" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" s="13">
-      <c r="A1" s="14" t="inlineStr">
-        <is>
-          <t>Area de Experimentacao - Sprint 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="13">
-      <c r="A2" s="12" t="inlineStr">
-        <is>
-          <t>Conexao e Extracao de Dados</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1" s="13">
+    <row r="1" ht="21" customHeight="1" s="12">
+      <c r="A1" s="13" t="inlineStr">
+        <is>
+          <t>Área de Experimentação - Sprint 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="12">
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>Conexão e Extração de Dados</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4" ht="18.75" customHeight="1" s="12">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>REQUISITOS PLANEJADOS</t>
@@ -623,7 +604,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Descricao</t>
+          <t>Descrição</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -638,12 +619,12 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>Data Inicio</t>
+          <t>Data Início</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Data Conclusao</t>
+          <t>Data Conclusão</t>
         </is>
       </c>
     </row>
@@ -655,7 +636,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Conexao SQL Server</t>
+          <t>Conexão SQL Server</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -670,7 +651,7 @@
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -692,7 +673,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Script de Extracao</t>
+          <t>Script de Extração</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -707,7 +688,7 @@
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -729,12 +710,12 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Geracao de Excel</t>
+          <t>Geração de Excel</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Gerar relatorio automatizado em formato Excel</t>
+          <t>Gerar relatório automatizado em formato Excel</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -744,7 +725,7 @@
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -758,10 +739,11 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="13">
+    <row r="9"/>
+    <row r="10" ht="18.75" customHeight="1" s="12">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>EVIDENCIAS DA EXECUCAO</t>
+          <t>EVIDÊNCIAS DA EXECUÇÃO</t>
         </is>
       </c>
     </row>
@@ -778,7 +760,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Descricao</t>
+          <t>Descrição</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -805,7 +787,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Teste de conexao via Python</t>
+          <t>Teste de conexão via Python</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -815,7 +797,7 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Conexao OK</t>
+          <t>Conexão OK</t>
         </is>
       </c>
     </row>
@@ -859,7 +841,7 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>Script de extracao rodando</t>
+          <t>Script de extração rodando</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
@@ -881,7 +863,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Codigo</t>
+          <t>Código</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -927,17 +909,18 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="18.75" customHeight="1" s="13">
+    <row r="17"/>
+    <row r="18" ht="18.75" customHeight="1" s="12">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>RESULTADOS ALCANCADOS</t>
+          <t>RESULTADOS ALCANÇADOS</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>Metrica</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -959,22 +942,22 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Tempo de geracao</t>
+          <t>Tempo de geração</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>~30 min/condominio</t>
+          <t>~30 min/condomínio</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>~4 segundos/condominio</t>
+          <t>~4 segundos/condomínio</t>
         </is>
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>99% mais rapido</t>
+          <t>99% mais rápido</t>
         </is>
       </c>
     </row>
@@ -986,12 +969,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Necessario</t>
+          <t>Necessário</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Dados ja estruturados</t>
+          <t>Dados já estruturados</t>
         </is>
       </c>
       <c r="D21" s="4" t="inlineStr">
@@ -1022,7 +1005,8 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="18.75" customHeight="1" s="13">
+    <row r="23"/>
+    <row r="24" ht="18.75" customHeight="1" s="12">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>RETROSPECTIVA DA SPRINT</t>
@@ -1037,7 +1021,7 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>Descricao</t>
+          <t>Descrição</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1033,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Conexao com SQL Server via Python funcionando</t>
+          <t>Conexão com SQL Server via Python funcionando</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1045,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Extracao de 2.762 registros em segundos</t>
+          <t>Extração de 2.762 registros em segundos</t>
         </is>
       </c>
     </row>
@@ -1073,7 +1057,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Geracao automatica de Excel estruturado</t>
+          <t>Geração automática de Excel estruturado</t>
         </is>
       </c>
     </row>
@@ -1085,7 +1069,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Lista de condominios configuravel via Excel</t>
+          <t>Lista de condomínios configurável via Excel</t>
         </is>
       </c>
     </row>
@@ -1109,38 +1093,38 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Indicador de situacao da unidade (adimplente/inadimplente)</t>
+          <t>Indicador de situação da unidade (adimplente/inadimplente)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>Nao validado (insight)</t>
+          <t>Não validado (insight)</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Ao analisar o tratamento manual, percebi que nao era possivel separar as unidades de forma consolidada</t>
+          <t>Ao analisar o tratamento manual, percebi que não era possível separar as unidades de forma consolidada</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
         <is>
-          <t>Nao validado (insight)</t>
+          <t>Não validado (insight)</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Nao era facil identificar se uma unidade era adimplente ou inadimplente no relatorio bruto</t>
+          <t>Não era fácil identificar se uma unidade era adimplente ou inadimplente no relatório bruto</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>Nao validado (insight)</t>
+          <t>Não validado (insight)</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1152,36 +1136,36 @@
     <row r="35">
       <c r="A35" s="7" t="inlineStr">
         <is>
-          <t>Licoes aprendidas</t>
+          <t>Lições aprendidas</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>Variaveis de ambiente (.env) facilitam configuracao segura</t>
+          <t>Variáveis de ambiente (.env) facilitam configuração segura</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="7" t="inlineStr">
         <is>
-          <t>Licoes aprendidas</t>
+          <t>Lições aprendidas</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Separar teste de conexao ajuda no debug</t>
+          <t>Separar teste de conexão ajuda no debug</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="inlineStr">
         <is>
-          <t>Licoes aprendidas</t>
+          <t>Lições aprendidas</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Parametrizar via Excel da flexibilidade sem alterar codigo</t>
+          <t>Parametrizar via Excel dá flexibilidade sem alterar código</t>
         </is>
       </c>
     </row>
@@ -1202,45 +1186,46 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" style="13" min="1" max="1"/>
-    <col width="52.140625" bestFit="1" customWidth="1" style="13" min="2" max="2"/>
-    <col width="55" customWidth="1" style="13" min="3" max="3"/>
-    <col width="25" customWidth="1" style="13" min="4" max="5"/>
-    <col width="15" customWidth="1" style="13" min="6" max="7"/>
+    <col width="22" customWidth="1" style="12" min="1" max="1"/>
+    <col width="52.140625" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="55" customWidth="1" style="12" min="3" max="3"/>
+    <col width="25" customWidth="1" style="12" min="4" max="5"/>
+    <col width="15" customWidth="1" style="12" min="6" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" s="13">
-      <c r="A1" s="14" t="inlineStr">
-        <is>
-          <t>Area de Experimentacao - Sprint 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="13">
-      <c r="A2" s="12" t="inlineStr">
-        <is>
-          <t>ETL e Consolidacao de Dados</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1" s="13">
-      <c r="A4" s="9" t="inlineStr">
+    <row r="1" ht="21" customHeight="1" s="12">
+      <c r="A1" s="13" t="inlineStr">
+        <is>
+          <t>Área de Experimentação - Sprint 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="12">
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>ETL e Consolidação de Dados</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4" ht="18.75" customHeight="1" s="12">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>REQUISITOS PLANEJADOS</t>
         </is>
       </c>
-      <c r="B4" s="10" t="n"/>
-      <c r="C4" s="10" t="n"/>
-      <c r="D4" s="10" t="n"/>
-      <c r="E4" s="10" t="n"/>
-      <c r="F4" s="10" t="n"/>
-      <c r="G4" s="10" t="n"/>
+      <c r="B4" s="9" t="n"/>
+      <c r="C4" s="9" t="n"/>
+      <c r="D4" s="9" t="n"/>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+      <c r="G4" s="9" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -1255,7 +1240,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Descricao</t>
+          <t>Descrição</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -1270,12 +1255,12 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>Data Inicio</t>
+          <t>Data Início</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Data Conclusao</t>
+          <t>Data Conclusão</t>
         </is>
       </c>
     </row>
@@ -1287,12 +1272,12 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Relatorio Individual</t>
+          <t>Relatório Individual</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Melhorar relatorio por unidade (2 abas: Detalhado + Resumo)</t>
+          <t>Melhorar relatório por unidade (2 abas: Detalhado + Resumo)</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -1302,7 +1287,7 @@
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -1324,7 +1309,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Relatorio Consolidado</t>
+          <t>Relatório Consolidado</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -1339,7 +1324,7 @@
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -1361,7 +1346,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Instalacao Airflow</t>
+          <t>Instalação Airflow</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1376,7 +1361,7 @@
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -1398,12 +1383,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Validacao Dados</t>
+          <t>Validação Dados</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Testar queries comparando com relatorio do sistema</t>
+          <t>Testar queries comparando com relatório do sistema</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -1413,7 +1398,7 @@
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Concluído</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
@@ -1428,26 +1413,26 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="n"/>
-      <c r="B10" s="10" t="n"/>
-      <c r="C10" s="10" t="n"/>
-      <c r="D10" s="10" t="n"/>
-      <c r="E10" s="10" t="n"/>
-      <c r="F10" s="10" t="n"/>
-      <c r="G10" s="10" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1" s="13">
-      <c r="A11" s="9" t="inlineStr">
-        <is>
-          <t>EVIDENCIAS DA EXECUCAO</t>
-        </is>
-      </c>
-      <c r="B11" s="10" t="n"/>
-      <c r="C11" s="10" t="n"/>
-      <c r="D11" s="10" t="n"/>
-      <c r="E11" s="10" t="n"/>
-      <c r="F11" s="10" t="n"/>
-      <c r="G11" s="10" t="n"/>
+      <c r="A10" s="9" t="n"/>
+      <c r="B10" s="9" t="n"/>
+      <c r="C10" s="9" t="n"/>
+      <c r="D10" s="9" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+      <c r="G10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" s="12">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>EVIDÊNCIAS DA EXECUÇÃO</t>
+        </is>
+      </c>
+      <c r="B11" s="9" t="n"/>
+      <c r="C11" s="9" t="n"/>
+      <c r="D11" s="9" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+      <c r="G11" s="9" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -1462,7 +1447,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Descricao</t>
+          <t>Descrição</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -1475,8 +1460,8 @@
           <t>Resultado</t>
         </is>
       </c>
-      <c r="F12" s="10" t="n"/>
-      <c r="G12" s="10" t="n"/>
+      <c r="F12" s="9" t="n"/>
+      <c r="G12" s="9" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -1491,7 +1476,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>Relatorio detalhado por boleto</t>
+          <t>Relatório detalhado por boleto</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
@@ -1504,8 +1489,8 @@
           <t>2.762 registros</t>
         </is>
       </c>
-      <c r="F13" s="10" t="n"/>
-      <c r="G13" s="10" t="n"/>
+      <c r="F13" s="9" t="n"/>
+      <c r="G13" s="9" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -1533,8 +1518,8 @@
           <t>552 unidades</t>
         </is>
       </c>
-      <c r="F14" s="10" t="n"/>
-      <c r="G14" s="10" t="n"/>
+      <c r="F14" s="9" t="n"/>
+      <c r="G14" s="9" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1559,11 +1544,11 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Metricas gerais</t>
-        </is>
-      </c>
-      <c r="F15" s="10" t="n"/>
-      <c r="G15" s="10" t="n"/>
+          <t>Métricas gerais</t>
+        </is>
+      </c>
+      <c r="F15" s="9" t="n"/>
+      <c r="G15" s="9" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
@@ -1578,7 +1563,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Dados por condominio</t>
+          <t>Dados por condomínio</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -1588,11 +1573,11 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>1 condominio</t>
-        </is>
-      </c>
-      <c r="F16" s="10" t="n"/>
-      <c r="G16" s="10" t="n"/>
+          <t>1 condomínio</t>
+        </is>
+      </c>
+      <c r="F16" s="9" t="n"/>
+      <c r="G16" s="9" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
@@ -1620,8 +1605,8 @@
           <t>110 unidades</t>
         </is>
       </c>
-      <c r="F17" s="10" t="n"/>
-      <c r="G17" s="10" t="n"/>
+      <c r="F17" s="9" t="n"/>
+      <c r="G17" s="9" t="n"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1676,8 +1661,8 @@
           <t>DAG configurada</t>
         </is>
       </c>
-      <c r="F19" s="10" t="n"/>
-      <c r="G19" s="10" t="n"/>
+      <c r="F19" s="9" t="n"/>
+      <c r="G19" s="9" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
@@ -1687,12 +1672,12 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Comparacao</t>
+          <t>Comparação</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>Validacao rec10.xlsx (relatório do sistema) vs banco</t>
+          <t>Validação rec10.xlsx (relatório do sistema) vs banco</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -1705,35 +1690,35 @@
           <t>100% bateu</t>
         </is>
       </c>
-      <c r="F20" s="10" t="n"/>
-      <c r="G20" s="10" t="n"/>
-    </row>
-    <row r="21" ht="18.75" customHeight="1" s="13">
-      <c r="A21" s="10" t="n"/>
-      <c r="B21" s="10" t="n"/>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="10" t="n"/>
-      <c r="E21" s="10" t="n"/>
-      <c r="F21" s="10" t="n"/>
-      <c r="G21" s="10" t="n"/>
-    </row>
-    <row r="22" ht="18.75" customHeight="1" s="13">
-      <c r="A22" s="9" t="inlineStr">
-        <is>
-          <t>RESULTADOS ALCANCADOS</t>
-        </is>
-      </c>
-      <c r="B22" s="10" t="n"/>
-      <c r="C22" s="10" t="n"/>
-      <c r="D22" s="10" t="n"/>
-      <c r="E22" s="10" t="n"/>
-      <c r="F22" s="10" t="n"/>
-      <c r="G22" s="10" t="n"/>
+      <c r="F20" s="9" t="n"/>
+      <c r="G20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18.75" customHeight="1" s="12">
+      <c r="A21" s="9" t="n"/>
+      <c r="B21" s="9" t="n"/>
+      <c r="C21" s="9" t="n"/>
+      <c r="D21" s="9" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+      <c r="G21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="18.75" customHeight="1" s="12">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>RESULTADOS ALCANÇADOS</t>
+        </is>
+      </c>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="9" t="n"/>
+      <c r="D22" s="9" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+      <c r="G22" s="9" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Metrica</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -1741,11 +1726,11 @@
           <t>Valor</t>
         </is>
       </c>
-      <c r="C23" s="10" t="n"/>
-      <c r="D23" s="10" t="n"/>
-      <c r="E23" s="10" t="n"/>
-      <c r="F23" s="10" t="n"/>
-      <c r="G23" s="10" t="n"/>
+      <c r="C23" s="9" t="n"/>
+      <c r="D23" s="9" t="n"/>
+      <c r="E23" s="9" t="n"/>
+      <c r="F23" s="9" t="n"/>
+      <c r="G23" s="9" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
@@ -1758,11 +1743,11 @@
           <t>552</t>
         </is>
       </c>
-      <c r="C24" s="10" t="n"/>
-      <c r="D24" s="10" t="n"/>
-      <c r="E24" s="10" t="n"/>
-      <c r="F24" s="10" t="n"/>
-      <c r="G24" s="10" t="n"/>
+      <c r="C24" s="9" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="9" t="n"/>
+      <c r="F24" s="9" t="n"/>
+      <c r="G24" s="9" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
@@ -1775,11 +1760,11 @@
           <t>442 (80%)</t>
         </is>
       </c>
-      <c r="C25" s="10" t="n"/>
-      <c r="D25" s="10" t="n"/>
-      <c r="E25" s="10" t="n"/>
-      <c r="F25" s="10" t="n"/>
-      <c r="G25" s="10" t="n"/>
+      <c r="C25" s="9" t="n"/>
+      <c r="D25" s="9" t="n"/>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+      <c r="G25" s="9" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
@@ -1792,11 +1777,11 @@
           <t>110 (20%)</t>
         </is>
       </c>
-      <c r="C26" s="10" t="n"/>
-      <c r="D26" s="10" t="n"/>
-      <c r="E26" s="10" t="n"/>
-      <c r="F26" s="10" t="n"/>
-      <c r="G26" s="10" t="n"/>
+      <c r="C26" s="9" t="n"/>
+      <c r="D26" s="9" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+      <c r="G26" s="9" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
@@ -1809,16 +1794,16 @@
           <t>R$ 1.455.152,46</t>
         </is>
       </c>
-      <c r="C27" s="10" t="n"/>
-      <c r="D27" s="10" t="n"/>
-      <c r="E27" s="10" t="n"/>
-      <c r="F27" s="10" t="n"/>
-      <c r="G27" s="10" t="n"/>
+      <c r="C27" s="9" t="n"/>
+      <c r="D27" s="9" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+      <c r="G27" s="9" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Validacao de Dados</t>
+          <t>Validação de Dados</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1826,33 +1811,33 @@
           <t>100% correto</t>
         </is>
       </c>
-      <c r="C28" s="10" t="n"/>
-      <c r="D28" s="10" t="n"/>
-      <c r="E28" s="10" t="n"/>
-      <c r="F28" s="10" t="n"/>
-      <c r="G28" s="10" t="n"/>
-    </row>
-    <row r="29" ht="18.75" customHeight="1" s="13">
-      <c r="A29" s="11" t="n"/>
-      <c r="B29" s="10" t="n"/>
-      <c r="C29" s="10" t="n"/>
-      <c r="D29" s="10" t="n"/>
-      <c r="E29" s="10" t="n"/>
-      <c r="F29" s="10" t="n"/>
-      <c r="G29" s="10" t="n"/>
-    </row>
-    <row r="30" ht="18.75" customHeight="1" s="13">
-      <c r="A30" s="9" t="inlineStr">
+      <c r="C28" s="9" t="n"/>
+      <c r="D28" s="9" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+      <c r="G28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18.75" customHeight="1" s="12">
+      <c r="A29" s="10" t="n"/>
+      <c r="B29" s="9" t="n"/>
+      <c r="C29" s="9" t="n"/>
+      <c r="D29" s="9" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+      <c r="G29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18.75" customHeight="1" s="12">
+      <c r="A30" s="8" t="inlineStr">
         <is>
           <t>RETROSPECTIVA DA SPRINT</t>
         </is>
       </c>
-      <c r="B30" s="10" t="n"/>
-      <c r="C30" s="10" t="n"/>
-      <c r="D30" s="10" t="n"/>
-      <c r="E30" s="10" t="n"/>
-      <c r="F30" s="10" t="n"/>
-      <c r="G30" s="10" t="n"/>
+      <c r="B30" s="9" t="n"/>
+      <c r="C30" s="9" t="n"/>
+      <c r="D30" s="9" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+      <c r="G30" s="9" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
@@ -1862,14 +1847,14 @@
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>Descricao</t>
-        </is>
-      </c>
-      <c r="C31" s="10" t="n"/>
-      <c r="D31" s="10" t="n"/>
-      <c r="E31" s="10" t="n"/>
-      <c r="F31" s="10" t="n"/>
-      <c r="G31" s="10" t="n"/>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="C31" s="9" t="n"/>
+      <c r="D31" s="9" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+      <c r="G31" s="9" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
@@ -1879,14 +1864,14 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Relatorio individual com resumo por unidade</t>
-        </is>
-      </c>
-      <c r="C32" s="10" t="n"/>
-      <c r="D32" s="10" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-      <c r="G32" s="10" t="n"/>
+          <t>Relatório individual com resumo por unidade</t>
+        </is>
+      </c>
+      <c r="C32" s="9" t="n"/>
+      <c r="D32" s="9" t="n"/>
+      <c r="E32" s="9" t="n"/>
+      <c r="F32" s="9" t="n"/>
+      <c r="G32" s="9" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -1896,14 +1881,14 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Consolidado com visao geral de inadimplencia</t>
-        </is>
-      </c>
-      <c r="C33" s="10" t="n"/>
-      <c r="D33" s="10" t="n"/>
-      <c r="E33" s="10" t="n"/>
-      <c r="F33" s="10" t="n"/>
-      <c r="G33" s="10" t="n"/>
+          <t>Consolidado com visão geral de inadimplência</t>
+        </is>
+      </c>
+      <c r="C33" s="9" t="n"/>
+      <c r="D33" s="9" t="n"/>
+      <c r="E33" s="9" t="n"/>
+      <c r="F33" s="9" t="n"/>
+      <c r="G33" s="9" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
@@ -1916,11 +1901,11 @@
           <t>Airflow instalado e configurado via Docker</t>
         </is>
       </c>
-      <c r="C34" s="10" t="n"/>
-      <c r="D34" s="10" t="n"/>
-      <c r="E34" s="10" t="n"/>
-      <c r="F34" s="10" t="n"/>
-      <c r="G34" s="10" t="n"/>
+      <c r="C34" s="9" t="n"/>
+      <c r="D34" s="9" t="n"/>
+      <c r="E34" s="9" t="n"/>
+      <c r="F34" s="9" t="n"/>
+      <c r="G34" s="9" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
@@ -1930,14 +1915,14 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>Validacao dos dados bateu 100% com sistema</t>
-        </is>
-      </c>
-      <c r="C35" s="10" t="n"/>
-      <c r="D35" s="10" t="n"/>
-      <c r="E35" s="10" t="n"/>
-      <c r="F35" s="10" t="n"/>
-      <c r="G35" s="10" t="n"/>
+          <t>Validação dos dados bateu 100% com sistema</t>
+        </is>
+      </c>
+      <c r="C35" s="9" t="n"/>
+      <c r="D35" s="9" t="n"/>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+      <c r="G35" s="9" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="inlineStr">
@@ -1947,14 +1932,14 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Adicionar mais condominios ao teste</t>
-        </is>
-      </c>
-      <c r="C36" s="10" t="n"/>
-      <c r="D36" s="10" t="n"/>
-      <c r="E36" s="10" t="n"/>
-      <c r="F36" s="10" t="n"/>
-      <c r="G36" s="10" t="n"/>
+          <t>Adicionar mais condomínios ao teste</t>
+        </is>
+      </c>
+      <c r="C36" s="9" t="n"/>
+      <c r="D36" s="9" t="n"/>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+      <c r="G36" s="9" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="inlineStr">
@@ -1964,36 +1949,36 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Automatizar envio de email com relatorios</t>
-        </is>
-      </c>
-      <c r="C37" s="10" t="n"/>
-      <c r="D37" s="10" t="n"/>
-      <c r="E37" s="10" t="n"/>
-      <c r="F37" s="10" t="n"/>
-      <c r="G37" s="10" t="n"/>
+          <t>Automatizar envio de email com relatórios</t>
+        </is>
+      </c>
+      <c r="C37" s="9" t="n"/>
+      <c r="D37" s="9" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+      <c r="G37" s="9" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="7" t="inlineStr">
         <is>
-          <t>Licoes aprendidas</t>
+          <t>Lições aprendidas</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Docker facilita instalacao do Airflow</t>
-        </is>
-      </c>
-      <c r="C38" s="10" t="n"/>
-      <c r="D38" s="10" t="n"/>
-      <c r="E38" s="10" t="n"/>
-      <c r="F38" s="10" t="n"/>
-      <c r="G38" s="10" t="n"/>
+          <t>Docker facilita instalação do Airflow</t>
+        </is>
+      </c>
+      <c r="C38" s="9" t="n"/>
+      <c r="D38" s="9" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+      <c r="G38" s="9" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="7" t="inlineStr">
         <is>
-          <t>Licoes aprendidas</t>
+          <t>Lições aprendidas</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -2001,120 +1986,120 @@
           <t>Validar dados com arquivo do sistema garante qualidade</t>
         </is>
       </c>
-      <c r="C39" s="10" t="n"/>
-      <c r="D39" s="10" t="n"/>
-      <c r="E39" s="10" t="n"/>
-      <c r="F39" s="10" t="n"/>
-      <c r="G39" s="10" t="n"/>
+      <c r="C39" s="9" t="n"/>
+      <c r="D39" s="9" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+      <c r="G39" s="9" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="n"/>
-      <c r="B40" s="10" t="n"/>
-      <c r="C40" s="10" t="n"/>
-      <c r="D40" s="10" t="n"/>
-      <c r="E40" s="10" t="n"/>
-      <c r="F40" s="10" t="n"/>
-      <c r="G40" s="10" t="n"/>
+      <c r="A40" s="9" t="n"/>
+      <c r="B40" s="9" t="n"/>
+      <c r="C40" s="9" t="n"/>
+      <c r="D40" s="9" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+      <c r="G40" s="9" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="n"/>
-      <c r="B41" s="10" t="n"/>
-      <c r="C41" s="10" t="n"/>
-      <c r="D41" s="10" t="n"/>
-      <c r="E41" s="10" t="n"/>
-      <c r="F41" s="10" t="n"/>
-      <c r="G41" s="10" t="n"/>
+      <c r="A41" s="9" t="n"/>
+      <c r="B41" s="9" t="n"/>
+      <c r="C41" s="9" t="n"/>
+      <c r="D41" s="9" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+      <c r="G41" s="9" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="n"/>
-      <c r="B42" s="10" t="n"/>
-      <c r="C42" s="10" t="n"/>
-      <c r="D42" s="10" t="n"/>
-      <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
-      <c r="G42" s="10" t="n"/>
+      <c r="A42" s="9" t="n"/>
+      <c r="B42" s="9" t="n"/>
+      <c r="C42" s="9" t="n"/>
+      <c r="D42" s="9" t="n"/>
+      <c r="E42" s="9" t="n"/>
+      <c r="F42" s="9" t="n"/>
+      <c r="G42" s="9" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="10" t="n"/>
-      <c r="B43" s="10" t="n"/>
-      <c r="C43" s="10" t="n"/>
-      <c r="D43" s="10" t="n"/>
-      <c r="E43" s="10" t="n"/>
-      <c r="F43" s="10" t="n"/>
-      <c r="G43" s="10" t="n"/>
+      <c r="A43" s="9" t="n"/>
+      <c r="B43" s="9" t="n"/>
+      <c r="C43" s="9" t="n"/>
+      <c r="D43" s="9" t="n"/>
+      <c r="E43" s="9" t="n"/>
+      <c r="F43" s="9" t="n"/>
+      <c r="G43" s="9" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="10" t="n"/>
-      <c r="B44" s="10" t="n"/>
-      <c r="C44" s="10" t="n"/>
-      <c r="D44" s="10" t="n"/>
-      <c r="E44" s="10" t="n"/>
-      <c r="F44" s="10" t="n"/>
-      <c r="G44" s="10" t="n"/>
+      <c r="A44" s="9" t="n"/>
+      <c r="B44" s="9" t="n"/>
+      <c r="C44" s="9" t="n"/>
+      <c r="D44" s="9" t="n"/>
+      <c r="E44" s="9" t="n"/>
+      <c r="F44" s="9" t="n"/>
+      <c r="G44" s="9" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="10" t="n"/>
-      <c r="B45" s="10" t="n"/>
-      <c r="C45" s="10" t="n"/>
-      <c r="D45" s="10" t="n"/>
-      <c r="E45" s="10" t="n"/>
-      <c r="F45" s="10" t="n"/>
-      <c r="G45" s="10" t="n"/>
+      <c r="A45" s="9" t="n"/>
+      <c r="B45" s="9" t="n"/>
+      <c r="C45" s="9" t="n"/>
+      <c r="D45" s="9" t="n"/>
+      <c r="E45" s="9" t="n"/>
+      <c r="F45" s="9" t="n"/>
+      <c r="G45" s="9" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="10" t="n"/>
-      <c r="B46" s="10" t="n"/>
-      <c r="C46" s="10" t="n"/>
-      <c r="D46" s="10" t="n"/>
-      <c r="E46" s="10" t="n"/>
-      <c r="F46" s="10" t="n"/>
-      <c r="G46" s="10" t="n"/>
+      <c r="A46" s="9" t="n"/>
+      <c r="B46" s="9" t="n"/>
+      <c r="C46" s="9" t="n"/>
+      <c r="D46" s="9" t="n"/>
+      <c r="E46" s="9" t="n"/>
+      <c r="F46" s="9" t="n"/>
+      <c r="G46" s="9" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="10" t="n"/>
-      <c r="B47" s="10" t="n"/>
-      <c r="C47" s="10" t="n"/>
-      <c r="D47" s="10" t="n"/>
-      <c r="E47" s="10" t="n"/>
-      <c r="F47" s="10" t="n"/>
-      <c r="G47" s="10" t="n"/>
+      <c r="A47" s="9" t="n"/>
+      <c r="B47" s="9" t="n"/>
+      <c r="C47" s="9" t="n"/>
+      <c r="D47" s="9" t="n"/>
+      <c r="E47" s="9" t="n"/>
+      <c r="F47" s="9" t="n"/>
+      <c r="G47" s="9" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="10" t="n"/>
-      <c r="B48" s="10" t="n"/>
-      <c r="C48" s="10" t="n"/>
-      <c r="D48" s="10" t="n"/>
-      <c r="E48" s="10" t="n"/>
-      <c r="F48" s="10" t="n"/>
-      <c r="G48" s="10" t="n"/>
+      <c r="A48" s="9" t="n"/>
+      <c r="B48" s="9" t="n"/>
+      <c r="C48" s="9" t="n"/>
+      <c r="D48" s="9" t="n"/>
+      <c r="E48" s="9" t="n"/>
+      <c r="F48" s="9" t="n"/>
+      <c r="G48" s="9" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="10" t="n"/>
-      <c r="B49" s="10" t="n"/>
-      <c r="C49" s="10" t="n"/>
-      <c r="D49" s="10" t="n"/>
-      <c r="E49" s="10" t="n"/>
-      <c r="F49" s="10" t="n"/>
-      <c r="G49" s="10" t="n"/>
+      <c r="A49" s="9" t="n"/>
+      <c r="B49" s="9" t="n"/>
+      <c r="C49" s="9" t="n"/>
+      <c r="D49" s="9" t="n"/>
+      <c r="E49" s="9" t="n"/>
+      <c r="F49" s="9" t="n"/>
+      <c r="G49" s="9" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="n"/>
-      <c r="B50" s="10" t="n"/>
-      <c r="C50" s="10" t="n"/>
-      <c r="D50" s="10" t="n"/>
-      <c r="E50" s="10" t="n"/>
-      <c r="F50" s="10" t="n"/>
-      <c r="G50" s="10" t="n"/>
+      <c r="A50" s="9" t="n"/>
+      <c r="B50" s="9" t="n"/>
+      <c r="C50" s="9" t="n"/>
+      <c r="D50" s="9" t="n"/>
+      <c r="E50" s="9" t="n"/>
+      <c r="F50" s="9" t="n"/>
+      <c r="G50" s="9" t="n"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Licoes aprendidas</t>
+          <t>Lições aprendidas</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Adiantamos parte do Sprint 3 (DAG Airflow ja configurada)</t>
+          <t>Adiantamos parte do Sprint 3 (DAG Airflow já configurada)</t>
         </is>
       </c>
     </row>
@@ -2135,758 +2120,757 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" style="13" min="1" max="1"/>
-    <col width="52" customWidth="1" style="13" min="2" max="2"/>
-    <col width="55" customWidth="1" style="13" min="3" max="3"/>
-    <col width="30" customWidth="1" style="13" min="4" max="4"/>
-    <col width="20" customWidth="1" style="13" min="5" max="5"/>
-    <col width="15" customWidth="1" style="13" min="6" max="6"/>
-    <col width="15" customWidth="1" style="13" min="7" max="7"/>
+    <col width="22" customWidth="1" style="12" min="1" max="1"/>
+    <col width="71.85546875" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="55" customWidth="1" style="12" min="3" max="3"/>
+    <col width="30" customWidth="1" style="12" min="4" max="4"/>
+    <col width="20" customWidth="1" style="12" min="5" max="5"/>
+    <col width="15" customWidth="1" style="12" min="6" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" s="13">
-      <c r="A1" s="23" t="inlineStr">
-        <is>
-          <t>Area de Experimentacao - Sprint 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="13">
-      <c r="A2" s="24" t="inlineStr">
-        <is>
-          <t>Orquestracao e Automacao Completa</t>
+    <row r="1" ht="21" customHeight="1" s="12">
+      <c r="A1" s="22" t="inlineStr">
+        <is>
+          <t>Área de Experimentação - Sprint 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="12">
+      <c r="A2" s="23" t="inlineStr">
+        <is>
+          <t>Orquestração e Automação Completa</t>
         </is>
       </c>
     </row>
     <row r="3"/>
-    <row r="4" ht="18.75" customHeight="1" s="13">
-      <c r="A4" s="25" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1" s="12">
+      <c r="A4" s="14" t="inlineStr">
         <is>
           <t>REQUISITOS PLANEJADOS</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="26" t="inlineStr">
+      <c r="A5" s="17" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B5" s="26" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>Requisito</t>
         </is>
       </c>
-      <c r="C5" s="26" t="inlineStr">
-        <is>
-          <t>Descricao</t>
-        </is>
-      </c>
-      <c r="D5" s="26" t="inlineStr">
+      <c r="C5" s="17" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="D5" s="17" t="inlineStr">
         <is>
           <t>Prioridade</t>
         </is>
       </c>
-      <c r="E5" s="26" t="inlineStr">
+      <c r="E5" s="17" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F5" s="26" t="inlineStr">
-        <is>
-          <t>Data Inicio</t>
-        </is>
-      </c>
-      <c r="G5" s="26" t="inlineStr">
-        <is>
-          <t>Data Conclusao</t>
+      <c r="F5" s="17" t="inlineStr">
+        <is>
+          <t>Data Início</t>
+        </is>
+      </c>
+      <c r="G5" s="17" t="inlineStr">
+        <is>
+          <t>Data Conclusão</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="inlineStr">
+      <c r="A6" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B6" s="20" t="inlineStr">
-        <is>
-          <t>Integracao DAG Airflow</t>
-        </is>
-      </c>
-      <c r="C6" s="20" t="inlineStr">
+      <c r="B6" s="18" t="inlineStr">
+        <is>
+          <t>Integração DAG Airflow</t>
+        </is>
+      </c>
+      <c r="C6" s="18" t="inlineStr">
         <is>
           <t>Integrar DAG com scripts reais (extrair_relatorio.py e extrair_consolidado.py)</t>
         </is>
       </c>
-      <c r="D6" s="20" t="inlineStr">
+      <c r="D6" s="18" t="inlineStr">
         <is>
           <t>Alta</t>
         </is>
       </c>
-      <c r="E6" s="27" t="inlineStr">
-        <is>
-          <t>Concluido</t>
-        </is>
-      </c>
-      <c r="F6" s="20" t="inlineStr">
+      <c r="E6" s="19" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+      <c r="F6" s="18" t="inlineStr">
         <is>
           <t>01/02/2026</t>
         </is>
       </c>
-      <c r="G6" s="20" t="inlineStr">
+      <c r="G6" s="18" t="inlineStr">
         <is>
           <t>02/02/2026</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="20" t="inlineStr">
+      <c r="A7" s="18" t="inlineStr">
         <is>
           <t>R8</t>
         </is>
       </c>
-      <c r="B7" s="20" t="inlineStr">
+      <c r="B7" s="18" t="inlineStr">
         <is>
           <t>Envio por Email</t>
         </is>
       </c>
-      <c r="C7" s="20" t="inlineStr">
-        <is>
-          <t>Codigo SMTP implementado na DAG, em stand-by aguardando credenciais</t>
-        </is>
-      </c>
-      <c r="D7" s="20" t="inlineStr">
+      <c r="C7" s="18" t="inlineStr">
+        <is>
+          <t>Código SMTP implementado na DAG, em stand-by aguardando credenciais</t>
+        </is>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
         <is>
           <t>Media</t>
         </is>
       </c>
-      <c r="E7" s="28" t="inlineStr">
+      <c r="E7" s="20" t="inlineStr">
         <is>
           <t>Stand-by</t>
         </is>
       </c>
-      <c r="F7" s="20" t="inlineStr">
+      <c r="F7" s="18" t="inlineStr">
         <is>
           <t>22/02/2026</t>
         </is>
       </c>
-      <c r="G7" s="20" t="inlineStr">
+      <c r="G7" s="18" t="inlineStr">
         <is>
           <t>22/02/2026</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="20" t="inlineStr">
+      <c r="A8" s="18" t="inlineStr">
         <is>
           <t>R9</t>
         </is>
       </c>
-      <c r="B8" s="20" t="inlineStr">
+      <c r="B8" s="18" t="inlineStr">
         <is>
           <t>Dashboard Final</t>
         </is>
       </c>
-      <c r="C8" s="20" t="inlineStr">
-        <is>
-          <t>Aguardando definicao da diretoria sobre metricas necessarias</t>
-        </is>
-      </c>
-      <c r="D8" s="20" t="inlineStr">
+      <c r="C8" s="18" t="inlineStr">
+        <is>
+          <t>Aguardando definição da diretoria sobre métricas necessárias</t>
+        </is>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
         <is>
           <t>Baixa</t>
         </is>
       </c>
-      <c r="E8" s="28" t="inlineStr">
+      <c r="E8" s="20" t="inlineStr">
         <is>
           <t>Stand-by</t>
         </is>
       </c>
-      <c r="F8" s="20" t="inlineStr">
+      <c r="F8" s="18" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G8" s="20" t="inlineStr">
+      <c r="G8" s="18" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="9"/>
-    <row r="10" ht="18.75" customHeight="1" s="13">
-      <c r="A10" s="25" t="inlineStr">
-        <is>
-          <t>EVIDENCIAS DA EXECUCAO</t>
+    <row r="10" ht="18.75" customHeight="1" s="12">
+      <c r="A10" s="14" t="inlineStr">
+        <is>
+          <t>EVIDÊNCIAS DA EXECUÇÃO</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="26" t="inlineStr">
+      <c r="A11" s="17" t="inlineStr">
         <is>
           <t>Requisito</t>
         </is>
       </c>
-      <c r="B11" s="26" t="inlineStr">
+      <c r="B11" s="17" t="inlineStr">
         <is>
           <t>Tipo</t>
         </is>
       </c>
-      <c r="C11" s="26" t="inlineStr">
-        <is>
-          <t>Descricao</t>
-        </is>
-      </c>
-      <c r="D11" s="26" t="inlineStr">
+      <c r="C11" s="17" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="D11" s="17" t="inlineStr">
         <is>
           <t>Arquivo</t>
         </is>
       </c>
-      <c r="E11" s="26" t="inlineStr">
+      <c r="E11" s="17" t="inlineStr">
         <is>
           <t>Resultado</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="20" t="inlineStr">
+      <c r="A12" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B12" s="20" t="inlineStr">
+      <c r="B12" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C12" s="20" t="inlineStr">
-        <is>
-          <t>DAG Airflow com 3 execucoes success</t>
-        </is>
-      </c>
-      <c r="D12" s="20" t="inlineStr">
+      <c r="C12" s="18" t="inlineStr">
+        <is>
+          <t>DAG Airflow com 3 execuções success</t>
+        </is>
+      </c>
+      <c r="D12" s="18" t="inlineStr">
         <is>
           <t>Relatorios_Semanais.png</t>
         </is>
       </c>
-      <c r="E12" s="20" t="inlineStr">
-        <is>
-          <t>3 execucoes OK</t>
+      <c r="E12" s="18" t="inlineStr">
+        <is>
+          <t>3 execuções OK</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="20" t="inlineStr">
+      <c r="A13" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B13" s="20" t="inlineStr">
+      <c r="B13" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C13" s="20" t="inlineStr">
+      <c r="C13" s="18" t="inlineStr">
         <is>
           <t>DAG atualizada com task enviar_email</t>
         </is>
       </c>
-      <c r="D13" s="20" t="inlineStr">
+      <c r="D13" s="18" t="inlineStr">
         <is>
           <t>dag_atualizada.png</t>
         </is>
       </c>
-      <c r="E13" s="20" t="inlineStr">
+      <c r="E13" s="18" t="inlineStr">
         <is>
           <t>Pipeline completo</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="20" t="inlineStr">
+      <c r="A14" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B14" s="20" t="inlineStr">
+      <c r="B14" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C14" s="20" t="inlineStr">
-        <is>
-          <t>Relatorio individual gerado automaticamente</t>
-        </is>
-      </c>
-      <c r="D14" s="20" t="inlineStr">
+      <c r="C14" s="18" t="inlineStr">
+        <is>
+          <t>Relatório individual gerado automaticamente</t>
+        </is>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
         <is>
           <t>Individual_Detalhado.png</t>
         </is>
       </c>
-      <c r="E14" s="20" t="inlineStr">
+      <c r="E14" s="18" t="inlineStr">
         <is>
           <t>2.762 registros</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="20" t="inlineStr">
+      <c r="A15" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B15" s="20" t="inlineStr">
+      <c r="B15" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C15" s="20" t="inlineStr">
+      <c r="C15" s="18" t="inlineStr">
         <is>
           <t>Resumo por unidade gerado automaticamente</t>
         </is>
       </c>
-      <c r="D15" s="20" t="inlineStr">
+      <c r="D15" s="18" t="inlineStr">
         <is>
           <t>Individual_Resumo_por_Unidade.png</t>
         </is>
       </c>
-      <c r="E15" s="20" t="inlineStr">
+      <c r="E15" s="18" t="inlineStr">
         <is>
           <t>552 unidades</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="20" t="inlineStr">
+      <c r="A16" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B16" s="20" t="inlineStr">
+      <c r="B16" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C16" s="20" t="inlineStr">
+      <c r="C16" s="18" t="inlineStr">
         <is>
           <t>Consolidado resumo geral</t>
         </is>
       </c>
-      <c r="D16" s="20" t="inlineStr">
+      <c r="D16" s="18" t="inlineStr">
         <is>
           <t>Consolidado_Resumo_Geral.png</t>
         </is>
       </c>
-      <c r="E16" s="20" t="inlineStr">
-        <is>
-          <t>Metricas gerais</t>
+      <c r="E16" s="18" t="inlineStr">
+        <is>
+          <t>Métricas gerais</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="20" t="inlineStr">
+      <c r="A17" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B17" s="20" t="inlineStr">
+      <c r="B17" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C17" s="20" t="inlineStr">
-        <is>
-          <t>Consolidado por condominio</t>
-        </is>
-      </c>
-      <c r="D17" s="20" t="inlineStr">
+      <c r="C17" s="18" t="inlineStr">
+        <is>
+          <t>Consolidado por condomínio</t>
+        </is>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
         <is>
           <t>Consolidado_Por_Condominio.png</t>
         </is>
       </c>
-      <c r="E17" s="20" t="inlineStr">
-        <is>
-          <t>1 condominio</t>
+      <c r="E17" s="18" t="inlineStr">
+        <is>
+          <t>1 condomínio</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="20" t="inlineStr">
+      <c r="A18" s="18" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="B18" s="20" t="inlineStr">
+      <c r="B18" s="18" t="inlineStr">
         <is>
           <t>Screenshot</t>
         </is>
       </c>
-      <c r="C18" s="20" t="inlineStr">
+      <c r="C18" s="18" t="inlineStr">
         <is>
           <t>Consolidado inadimplentes</t>
         </is>
       </c>
-      <c r="D18" s="20" t="inlineStr">
+      <c r="D18" s="18" t="inlineStr">
         <is>
           <t>Consolidado_Inadimplentes.png</t>
         </is>
       </c>
-      <c r="E18" s="20" t="inlineStr">
+      <c r="E18" s="18" t="inlineStr">
         <is>
           <t>523 inadimplentes</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="20" t="inlineStr">
+      <c r="A19" s="18" t="inlineStr">
         <is>
           <t>R8</t>
         </is>
       </c>
-      <c r="B19" s="20" t="inlineStr">
-        <is>
-          <t>Codigo</t>
-        </is>
-      </c>
-      <c r="C19" s="20" t="inlineStr">
+      <c r="B19" s="18" t="inlineStr">
+        <is>
+          <t>Código</t>
+        </is>
+      </c>
+      <c r="C19" s="18" t="inlineStr">
         <is>
           <t>Task enviar_email com flag ENVIO_EMAIL_ATIVO</t>
         </is>
       </c>
-      <c r="D19" s="20" t="inlineStr">
+      <c r="D19" s="18" t="inlineStr">
         <is>
           <t>relatorios_semanais.py</t>
         </is>
       </c>
-      <c r="E19" s="20" t="inlineStr">
+      <c r="E19" s="18" t="inlineStr">
         <is>
           <t>Stand-by</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="20" t="inlineStr">
+      <c r="A20" s="18" t="inlineStr">
         <is>
           <t>R9</t>
         </is>
       </c>
-      <c r="B20" s="20" t="inlineStr">
-        <is>
-          <t>Decisao</t>
-        </is>
-      </c>
-      <c r="C20" s="20" t="inlineStr">
-        <is>
-          <t>Aguardando diretoria definir visualizacoes</t>
-        </is>
-      </c>
-      <c r="D20" s="20" t="inlineStr">
+      <c r="B20" s="18" t="inlineStr">
+        <is>
+          <t>Decisão</t>
+        </is>
+      </c>
+      <c r="C20" s="18" t="inlineStr">
+        <is>
+          <t>Aguardando diretoria definir visualizações</t>
+        </is>
+      </c>
+      <c r="D20" s="18" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E20" s="20" t="inlineStr">
+      <c r="E20" s="18" t="inlineStr">
         <is>
           <t>Stand-by</t>
         </is>
       </c>
     </row>
     <row r="21"/>
-    <row r="22" ht="18.75" customHeight="1" s="13">
-      <c r="A22" s="25" t="inlineStr">
-        <is>
-          <t>RESULTADOS ALCANCADOS</t>
+    <row r="22" ht="18.75" customHeight="1" s="12">
+      <c r="A22" s="14" t="inlineStr">
+        <is>
+          <t>RESULTADOS ALCANÇADOS</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="26" t="inlineStr">
-        <is>
-          <t>Metrica</t>
-        </is>
-      </c>
-      <c r="B23" s="26" t="inlineStr">
+      <c r="A23" s="17" t="inlineStr">
+        <is>
+          <t>Métrica</t>
+        </is>
+      </c>
+      <c r="B23" s="17" t="inlineStr">
         <is>
           <t>Valor</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="20" t="inlineStr">
-        <is>
-          <t>Execucoes automaticas</t>
-        </is>
-      </c>
-      <c r="B24" s="20" t="inlineStr">
+      <c r="A24" s="18" t="inlineStr">
+        <is>
+          <t>Execuções automáticas</t>
+        </is>
+      </c>
+      <c r="B24" s="18" t="inlineStr">
         <is>
           <t>2 (02/02 e 09/02)</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="20" t="inlineStr">
-        <is>
-          <t>Execucoes manuais</t>
-        </is>
-      </c>
-      <c r="B25" s="20" t="inlineStr">
+      <c r="A25" s="18" t="inlineStr">
+        <is>
+          <t>Execuções manuais</t>
+        </is>
+      </c>
+      <c r="B25" s="18" t="inlineStr">
         <is>
           <t>1 (22/02)</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="20" t="inlineStr">
-        <is>
-          <t>Tempo de execucao</t>
-        </is>
-      </c>
-      <c r="B26" s="20" t="inlineStr">
+      <c r="A26" s="18" t="inlineStr">
+        <is>
+          <t>Tempo de execução</t>
+        </is>
+      </c>
+      <c r="B26" s="18" t="inlineStr">
         <is>
           <t>9 segundos</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="20" t="inlineStr">
-        <is>
-          <t>Reducao de tempo</t>
-        </is>
-      </c>
-      <c r="B27" s="20" t="inlineStr">
+      <c r="A27" s="18" t="inlineStr">
+        <is>
+          <t>Redução de tempo</t>
+        </is>
+      </c>
+      <c r="B27" s="18" t="inlineStr">
         <is>
           <t>De 3-4 horas para 9 segundos (99.9%)</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="20" t="inlineStr">
+      <c r="A28" s="18" t="inlineStr">
         <is>
           <t>Falha identificada</t>
         </is>
       </c>
-      <c r="B28" s="20" t="inlineStr">
+      <c r="B28" s="18" t="inlineStr">
         <is>
           <t>16/02 - Docker Desktop fechado</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="20" t="inlineStr">
+      <c r="A29" s="18" t="inlineStr">
         <is>
           <t>R8 Email</t>
         </is>
       </c>
-      <c r="B29" s="20" t="inlineStr">
-        <is>
-          <t>Codigo pronto, aguardando SMTP</t>
+      <c r="B29" s="18" t="inlineStr">
+        <is>
+          <t>Código pronto, aguardando SMTP</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="20" t="inlineStr">
+      <c r="A30" s="18" t="inlineStr">
         <is>
           <t>R9 Dashboard</t>
         </is>
       </c>
-      <c r="B30" s="20" t="inlineStr">
-        <is>
-          <t>Aguardando definicao da diretoria</t>
+      <c r="B30" s="18" t="inlineStr">
+        <is>
+          <t>Aguardando definição da diretoria</t>
         </is>
       </c>
     </row>
     <row r="31"/>
-    <row r="32" ht="18.75" customHeight="1" s="13">
-      <c r="A32" s="25" t="inlineStr">
+    <row r="32" ht="18.75" customHeight="1" s="12">
+      <c r="A32" s="14" t="inlineStr">
         <is>
           <t>RETROSPECTIVA DA SPRINT</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="26" t="inlineStr">
+      <c r="A33" s="17" t="inlineStr">
         <is>
           <t>Categoria</t>
         </is>
       </c>
-      <c r="B33" s="26" t="inlineStr">
-        <is>
-          <t>Descricao</t>
+      <c r="B33" s="17" t="inlineStr">
+        <is>
+          <t>Descrição</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="27" t="inlineStr">
+      <c r="A34" s="19" t="inlineStr">
         <is>
           <t>O que funcionou</t>
         </is>
       </c>
-      <c r="B34" s="27" t="inlineStr">
+      <c r="B34" s="19" t="inlineStr">
         <is>
           <t>Pipeline completo executando via Airflow em 9 segundos</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="27" t="inlineStr">
+      <c r="A35" s="19" t="inlineStr">
         <is>
           <t>O que funcionou</t>
         </is>
       </c>
-      <c r="B35" s="27" t="inlineStr">
-        <is>
-          <t>Execucao automatica agendada funcionou na segunda 09/02 as 06:00</t>
+      <c r="B35" s="19" t="inlineStr">
+        <is>
+          <t>Execução automática agendada funcionou na segunda 09/02 as 06:00</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="27" t="inlineStr">
+      <c r="A36" s="19" t="inlineStr">
         <is>
           <t>O que funcionou</t>
         </is>
       </c>
-      <c r="B36" s="27" t="inlineStr">
+      <c r="B36" s="19" t="inlineStr">
         <is>
           <t>Dockerfile customizado com ODBC SQL Server operando corretamente</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="27" t="inlineStr">
+      <c r="A37" s="19" t="inlineStr">
         <is>
           <t>O que funcionou</t>
         </is>
       </c>
-      <c r="B37" s="27" t="inlineStr">
-        <is>
-          <t>Codigo de envio por email implementado e pronto para ativacao</t>
+      <c r="B37" s="19" t="inlineStr">
+        <is>
+          <t>Código de envio por email implementado e pronto para ativação</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="27" t="inlineStr">
+      <c r="A38" s="19" t="inlineStr">
         <is>
           <t>O que nao funcionou</t>
         </is>
       </c>
-      <c r="B38" s="27" t="inlineStr">
-        <is>
-          <t>Em 16/02 a execucao falhou pois Docker Desktop estava fechado</t>
+      <c r="B38" s="19" t="inlineStr">
+        <is>
+          <t>Em 16/02 a execução falhou pois Docker Desktop estava fechado</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
+      <c r="A39" s="20" t="inlineStr">
         <is>
           <t>Stand-by</t>
         </is>
       </c>
-      <c r="B39" s="28" t="inlineStr">
-        <is>
-          <t>R8: Envio por email - codigo pronto, aguardando credenciais SMTP</t>
+      <c r="B39" s="20" t="inlineStr">
+        <is>
+          <t>R8: Envio por email - código pronto, aguardando credenciais SMTP</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
+      <c r="A40" s="20" t="inlineStr">
         <is>
           <t>Stand-by</t>
         </is>
       </c>
-      <c r="B40" s="28" t="inlineStr">
-        <is>
-          <t>R9: Dashboard - aguardando diretoria definir metricas</t>
+      <c r="B40" s="20" t="inlineStr">
+        <is>
+          <t>R9: Dashboard - aguardando diretoria definir métricas</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="inlineStr">
+      <c r="A41" s="20" t="inlineStr">
         <is>
           <t>O que pode melhorar</t>
         </is>
       </c>
-      <c r="B41" s="28" t="inlineStr">
+      <c r="B41" s="20" t="inlineStr">
         <is>
           <t>Configurar Docker Desktop para iniciar com o Windows</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="inlineStr">
+      <c r="A42" s="20" t="inlineStr">
         <is>
           <t>O que pode melhorar</t>
         </is>
       </c>
-      <c r="B42" s="28" t="inlineStr">
-        <is>
-          <t>Cadastrar credenciais SMTP para ativar envio automatico</t>
+      <c r="B42" s="20" t="inlineStr">
+        <is>
+          <t>Cadastrar credenciais SMTP para ativar envio automático</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="29" t="inlineStr">
-        <is>
-          <t>Licoes aprendidas</t>
-        </is>
-      </c>
-      <c r="B43" s="29" t="inlineStr">
+      <c r="A43" s="21" t="inlineStr">
+        <is>
+          <t>Lições aprendidas</t>
+        </is>
+      </c>
+      <c r="B43" s="21" t="inlineStr">
         <is>
           <t>Docker Desktop precisa estar ativo para Airflow funcionar</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="29" t="inlineStr">
-        <is>
-          <t>Licoes aprendidas</t>
-        </is>
-      </c>
-      <c r="B44" s="29" t="inlineStr">
+      <c r="A44" s="21" t="inlineStr">
+        <is>
+          <t>Lições aprendidas</t>
+        </is>
+      </c>
+      <c r="B44" s="21" t="inlineStr">
         <is>
           <t>Docker com volumes permite integrar scripts externos ao Airflow</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="29" t="inlineStr">
-        <is>
-          <t>Licoes aprendidas</t>
-        </is>
-      </c>
-      <c r="B45" s="29" t="inlineStr">
-        <is>
-          <t>Driver ODBC no Linux requer configuracao especifica via Dockerfile</t>
+      <c r="A45" s="21" t="inlineStr">
+        <is>
+          <t>Lições aprendidas</t>
+        </is>
+      </c>
+      <c r="B45" s="21" t="inlineStr">
+        <is>
+          <t>Driver ODBC no Linux requer configuração específica via Dockerfile</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="29" t="inlineStr">
-        <is>
-          <t>Licoes aprendidas</t>
-        </is>
-      </c>
-      <c r="B46" s="29" t="inlineStr">
-        <is>
-          <t>Funcionalidades em stand-by com flag permite ativacao futura sem retrabalho</t>
+      <c r="A46" s="21" t="inlineStr">
+        <is>
+          <t>Lições aprendidas</t>
+        </is>
+      </c>
+      <c r="B46" s="21" t="inlineStr">
+        <is>
+          <t>Funcionalidades em stand-by com flag permite ativação futura sem retrabalho</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="29" t="inlineStr">
-        <is>
-          <t>Licoes aprendidas</t>
-        </is>
-      </c>
-      <c r="B47" s="29" t="inlineStr">
-        <is>
-          <t>Pipeline de 3-4 horas reduzido para 9 segundos (99.9% mais rapido)</t>
+      <c r="A47" s="21" t="inlineStr">
+        <is>
+          <t>Lições aprendidas</t>
+        </is>
+      </c>
+      <c r="B47" s="21" t="inlineStr">
+        <is>
+          <t>Pipeline de 3-4 horas reduzido para 9 segundos (99.9% mais rápido)</t>
         </is>
       </c>
     </row>

</xml_diff>